<commit_message>
dependency injection - xml, annotation, java config
</commit_message>
<xml_diff>
--- a/pocs.xlsx
+++ b/pocs.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB6DF38-24F1-4B56-BE66-9DA8F19562EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F4CB72-188E-4400-AE70-D743FD8A34B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="pocs" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>

</xml_diff>